<commit_message>
Add ScreenshotUtils class for capturing screenshots
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2025\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5A328C-A627-436E-877D-C48EC82C5423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEEAC0F-FDF3-407E-88AC-86293D6D48F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>testname</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -412,7 +415,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +453,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Integrated Data Provider with the framework for parameterized testing
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2025\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEEAC0F-FDF3-407E-88AC-86293D6D48F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863CBCDC-2ECF-47A8-AC3E-BF2FD0EDE11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
   </bookViews>
   <sheets>
-    <sheet name="Runner" sheetId="1" r:id="rId1"/>
+    <sheet name="Tests" sheetId="1" r:id="rId1"/>
+    <sheet name="DataProviderTests" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
   <si>
     <t>testname</t>
   </si>
@@ -58,14 +59,40 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>adminnn</t>
+  </si>
+  <si>
+    <t>admin12345</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,9 +120,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -414,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7BD656-95B7-4781-86DD-3AA35FF95671}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,20 +458,20 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -470,7 +500,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -483,4 +513,124 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDD0107-66D8-4E03-8137-EBB5C3C1F685}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented RetryAnalyzer Listener for retrying failed tests
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2025\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863CBCDC-2ECF-47A8-AC3E-BF2FD0EDE11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E21C38C-19EF-4DC5-9D54-667A74DEB03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
   <si>
     <t>testname</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>admin12345</t>
+  </si>
+  <si>
+    <t>testOne</t>
+  </si>
+  <si>
+    <t>testTwo</t>
+  </si>
+  <si>
+    <t>Google search Test</t>
   </si>
 </sst>
 </file>
@@ -442,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7BD656-95B7-4781-86DD-3AA35FF95671}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,12 +509,46 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
         <v>1</v>
       </c>
     </row>
@@ -520,7 +563,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +594,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -565,7 +608,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
@@ -579,7 +622,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -593,7 +636,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -621,7 +664,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Enabled parallel cross-browser testing to optimize execution time and coverage
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2025\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E21C38C-19EF-4DC5-9D54-667A74DEB03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03238A87-7066-4724-8187-CB25FA934D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
   <si>
     <t>testname</t>
   </si>
@@ -86,6 +86,18 @@
   </si>
   <si>
     <t>Google search Test</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>edge</t>
   </si>
 </sst>
 </file>
@@ -454,7 +466,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +521,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -560,22 +572,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDD0107-66D8-4E03-8137-EBB5C3C1F685}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -583,27 +596,33 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -611,65 +630,108 @@
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new test case for Amazon application - navigateToTabletsPageViaHamburgerMenuTest
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2025\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03238A87-7066-4724-8187-CB25FA934D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236AE4C6-BDDF-433A-BA6F-06AC66A3C288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="27">
   <si>
     <t>testname</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>edge</t>
+  </si>
+  <si>
+    <t>navigateToTabletsPageViaHamburgerMenuTest</t>
+  </si>
+  <si>
+    <t>This testcase checks navigation to Tablets Page Via the Hamburger menu options</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -141,12 +150,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -463,16 +475,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7BD656-95B7-4781-86DD-3AA35FF95671}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" style="1" bestFit="1" customWidth="1"/>
@@ -504,7 +516,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -521,7 +533,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -562,6 +574,23 @@
       </c>
       <c r="E5" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -572,20 +601,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDD0107-66D8-4E03-8137-EBB5C3C1F685}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -610,7 +641,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>21</v>
@@ -627,7 +658,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>23</v>
@@ -644,7 +675,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>22</v>
@@ -661,7 +692,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>21</v>
@@ -706,7 +737,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>23</v>
@@ -723,7 +754,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>22</v>
@@ -733,6 +764,23 @@
       </c>
       <c r="E9" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added DynamicXpathUtils class for runtime xPath generation using String.format
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2025\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236AE4C6-BDDF-433A-BA6F-06AC66A3C288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D53AE8-00FE-4ADA-B508-0846B502EADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
   </bookViews>
@@ -478,7 +478,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E5" sqref="E5:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code updated to handle CAPTCHA in amazon application
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2025\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D53AE8-00FE-4ADA-B508-0846B502EADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422BD755-27E6-4ED5-A38A-5AB1240F9592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
   </bookViews>
@@ -478,7 +478,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added custom annotations to assign Authors & Test Categories in reports
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2025\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422BD755-27E6-4ED5-A38A-5AB1240F9592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5B586A-E3CA-453D-AF02-EB9F9FD15BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
   </bookViews>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented password masking using Base64 encoding & decoding
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2025\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5B586A-E3CA-453D-AF02-EB9F9FD15BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5C8BD1-FD7C-4093-ACCE-ED0977109E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="26">
   <si>
     <t>testname</t>
   </si>
@@ -70,15 +70,9 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>admin123</t>
-  </si>
-  <si>
     <t>adminnn</t>
   </si>
   <si>
-    <t>admin12345</t>
-  </si>
-  <si>
     <t>testOne</t>
   </si>
   <si>
@@ -107,6 +101,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>YWRtaW4xMjM=</t>
   </si>
 </sst>
 </file>
@@ -150,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -160,6 +157,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7BD656-95B7-4781-86DD-3AA35FF95671}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,10 +495,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -509,14 +512,14 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -526,10 +529,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -543,11 +546,11 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
@@ -560,11 +563,11 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
@@ -577,14 +580,14 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>25</v>
+      <c r="A6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -603,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDD0107-66D8-4E03-8137-EBB5C3C1F685}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +616,7 @@
     <col min="2" max="2" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
@@ -627,7 +630,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>11</v>
@@ -641,16 +644,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -658,16 +661,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -678,13 +681,13 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -695,13 +698,13 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -715,7 +718,7 @@
         <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -726,10 +729,10 @@
         <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -740,13 +743,13 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -757,30 +760,30 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created DriverFactory class to manager Browser Invocation
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2025\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5C8BD1-FD7C-4093-ACCE-ED0977109E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A11188E-094D-4A28-9FD2-C0C99BC42793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="26">
   <si>
     <t>testname</t>
   </si>
@@ -481,7 +481,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +519,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -587,7 +587,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -604,10 +604,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDD0107-66D8-4E03-8137-EBB5C3C1F685}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +644,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>19</v>
@@ -661,7 +661,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>21</v>
@@ -774,7 +774,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>19</v>
@@ -783,6 +783,40 @@
         <v>24</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented ELK stack for RealTime Dashboard and monitoring
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2025\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBD06BF-4DDF-4F76-AA40-6887B99C42D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488D437C-964C-4A57-9622-21A4C4085C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="27">
   <si>
     <t>testname</t>
   </si>
@@ -483,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7BD656-95B7-4781-86DD-3AA35FF95671}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +593,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -607,10 +607,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDD0107-66D8-4E03-8137-EBB5C3C1F685}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,6 +817,61 @@
         <v>26</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new scripts and code changes
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2025\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488D437C-964C-4A57-9622-21A4C4085C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77061EC-42E9-484E-86D5-BA1C1C84EEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="24">
   <si>
     <t>testname</t>
   </si>
@@ -43,45 +43,9 @@
     <t>count</t>
   </si>
   <si>
-    <t>loginTestWithValidCredentials</t>
-  </si>
-  <si>
-    <t>loginTestWithInValidCredentials</t>
-  </si>
-  <si>
-    <t>This testcase is used to check if the test passes with valid credentails or not.</t>
-  </si>
-  <si>
-    <t>This testcase is used to check if the test failes with Invalid credentails or not.</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>adminnn</t>
-  </si>
-  <si>
-    <t>testOne</t>
-  </si>
-  <si>
-    <t>testTwo</t>
-  </si>
-  <si>
-    <t>Google search Test</t>
-  </si>
-  <si>
     <t>browser</t>
   </si>
   <si>
@@ -91,22 +55,49 @@
     <t>firefox</t>
   </si>
   <si>
-    <t>edge</t>
-  </si>
-  <si>
     <t>navigateToTabletsPageViaHamburgerMenuTest</t>
   </si>
   <si>
     <t>This testcase checks navigation to Tablets Page Via the Hamburger menu options</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>YWRtaW4xMjM=</t>
-  </si>
-  <si>
     <t>MicrosoftEdge</t>
+  </si>
+  <si>
+    <t>navigateToMensFashionPageViaHamburgerMenuTest</t>
+  </si>
+  <si>
+    <t>navigateToAmazonPrimeVideoPageViaHamburgerMenuTest</t>
+  </si>
+  <si>
+    <t>This testcase checks navigation to Men's Fashion Page Via the Hamburger menu options</t>
+  </si>
+  <si>
+    <t>This testcase checks navigation to Prime Video Page Via the Hamburger menu options</t>
+  </si>
+  <si>
+    <t>menuoption</t>
+  </si>
+  <si>
+    <t>submenuoption</t>
+  </si>
+  <si>
+    <t>Mobiles, Computers</t>
+  </si>
+  <si>
+    <t>Tablets</t>
+  </si>
+  <si>
+    <t>Men's Fashion</t>
+  </si>
+  <si>
+    <t>Jeans</t>
+  </si>
+  <si>
+    <t>Fire TV</t>
+  </si>
+  <si>
+    <t>Amazon Prime Video</t>
   </si>
 </sst>
 </file>
@@ -481,16 +472,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7BD656-95B7-4781-86DD-3AA35FF95671}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="80.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" style="1" bestFit="1" customWidth="1"/>
@@ -516,13 +507,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -533,16 +524,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -550,52 +541,18 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1">
         <v>1</v>
       </c>
     </row>
@@ -607,22 +564,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDD0107-66D8-4E03-8137-EBB5C3C1F685}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B17"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -633,246 +589,170 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>20</v>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix issue with ELK Dashboard index for updating testcase status
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2025\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77061EC-42E9-484E-86D5-BA1C1C84EEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D14EA64-FE33-41E8-B7F5-F4077B2D0E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{ECA42F6A-100D-4AAD-8B9C-50B122A37449}"/>
   </bookViews>
@@ -567,7 +567,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>